<commit_message>
update ServerStat Excel file
</commit_message>
<xml_diff>
--- a/BenchmarkRawData/ServerStat.xlsx
+++ b/BenchmarkRawData/ServerStat.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TwITe\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TwITe\Documents\BenchmarkRawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Go Server" sheetId="1" r:id="rId1"/>
     <sheet name="C++ Server" sheetId="2" r:id="rId2"/>
-    <sheet name="Bots Servers" sheetId="3" r:id="rId3"/>
+    <sheet name="Both Servers" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="CPPStat" localSheetId="1">'C++ Server'!$A$1:$B$537</definedName>
@@ -3474,7 +3474,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Bots Servers'!$B$3</c:f>
+              <c:f>'Both Servers'!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3495,7 +3495,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Bots Servers'!$A$4:$A$6</c:f>
+              <c:f>'Both Servers'!$A$4:$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -3512,7 +3512,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Bots Servers'!$B$4:$B$6</c:f>
+              <c:f>'Both Servers'!$B$4:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -3539,7 +3539,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Bots Servers'!$C$3</c:f>
+              <c:f>'Both Servers'!$C$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3560,7 +3560,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Bots Servers'!$A$4:$A$6</c:f>
+              <c:f>'Both Servers'!$A$4:$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -3577,7 +3577,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Bots Servers'!$C$4:$C$6</c:f>
+              <c:f>'Both Servers'!$C$4:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -3684,6 +3684,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time in milliseconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3877,7 +3933,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Bots Servers'!$B$8</c:f>
+              <c:f>'Both Servers'!$B$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3900,7 +3956,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Bots Servers'!$A$9:$A$37</c:f>
+              <c:f>'Both Servers'!$A$9:$A$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
@@ -3996,7 +4052,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Bots Servers'!$B$9:$B$37</c:f>
+              <c:f>'Both Servers'!$B$9:$B$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
@@ -4102,7 +4158,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Bots Servers'!$C$8</c:f>
+              <c:f>'Both Servers'!$C$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4125,7 +4181,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Bots Servers'!$A$9:$A$37</c:f>
+              <c:f>'Both Servers'!$A$9:$A$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
@@ -4221,7 +4277,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Bots Servers'!$C$9:$C$37</c:f>
+              <c:f>'Both Servers'!$C$9:$C$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
@@ -4341,6 +4397,73 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> clients</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.39477580927384076"/>
+              <c:y val="0.79592519685039353"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4406,6 +4529,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time in milliseconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4599,7 +4778,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Bots Servers'!$B$39</c:f>
+              <c:f>'Both Servers'!$B$39</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4622,7 +4801,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Bots Servers'!$A$40:$A$68</c:f>
+              <c:f>'Both Servers'!$A$40:$A$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
@@ -4718,7 +4897,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Bots Servers'!$B$40:$B$68</c:f>
+              <c:f>'Both Servers'!$B$40:$B$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
@@ -4824,7 +5003,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Bots Servers'!$C$39</c:f>
+              <c:f>'Both Servers'!$C$39</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4847,7 +5026,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Bots Servers'!$A$40:$A$68</c:f>
+              <c:f>'Both Servers'!$A$40:$A$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
@@ -4943,7 +5122,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Bots Servers'!$C$40:$C$68</c:f>
+              <c:f>'Both Servers'!$C$40:$C$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
@@ -5063,6 +5242,69 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of clients</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.39061614173228354"/>
+              <c:y val="0.80518445610965295"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -5128,6 +5370,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time in milliseconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -5321,7 +5619,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Bots Servers'!$B$70</c:f>
+              <c:f>'Both Servers'!$B$70</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5344,7 +5642,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Bots Servers'!$A$71:$A$99</c:f>
+              <c:f>'Both Servers'!$A$71:$A$99</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
@@ -5440,7 +5738,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Bots Servers'!$B$71:$B$99</c:f>
+              <c:f>'Both Servers'!$B$71:$B$99</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
@@ -5546,7 +5844,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Bots Servers'!$C$70</c:f>
+              <c:f>'Both Servers'!$C$70</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5569,7 +5867,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Bots Servers'!$A$71:$A$99</c:f>
+              <c:f>'Both Servers'!$A$71:$A$99</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
@@ -5665,7 +5963,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Bots Servers'!$C$71:$C$99</c:f>
+              <c:f>'Both Servers'!$C$71:$C$99</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
@@ -5785,6 +6083,69 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of clients</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.39027580927384076"/>
+              <c:y val="0.8190733449985419"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -5850,6 +6211,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time in milliseconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -6010,7 +6427,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6052,7 +6468,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Bots Servers'!$B$105</c:f>
+              <c:f>'Both Servers'!$B$105</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6073,7 +6489,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Bots Servers'!$A$106:$A$108</c:f>
+              <c:f>'Both Servers'!$A$106:$A$108</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -6090,7 +6506,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Bots Servers'!$B$106:$B$108</c:f>
+              <c:f>'Both Servers'!$B$106:$B$108</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -6117,7 +6533,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Bots Servers'!$C$105</c:f>
+              <c:f>'Both Servers'!$C$105</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6138,7 +6554,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Bots Servers'!$A$106:$A$108</c:f>
+              <c:f>'Both Servers'!$A$106:$A$108</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -6155,7 +6571,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Bots Servers'!$C$106:$C$108</c:f>
+              <c:f>'Both Servers'!$C$106:$C$108</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -6262,6 +6678,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time in milliseconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -6307,7 +6778,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13637,8 +14107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B537"/>
   <sheetViews>
-    <sheetView topLeftCell="A205" workbookViewId="0">
-      <selection activeCell="C223" sqref="C223"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17790,8 +18260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>